<commit_message>
Updated Excel with Actual Spent Time
Added Actual Spent Time for UC Settings Tab (Semester II)
</commit_message>
<xml_diff>
--- a/organization/Function Points.xlsx
+++ b/organization/Function Points.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>General Tab</t>
   </si>
@@ -346,7 +346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D1D95F4-5A3F-4E38-86A2-9CFE84944AF1}" type="CELLRANGE">
+                    <a:fld id="{6A56DAA6-D628-4A2B-9B66-C47D8964AF03}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -379,7 +379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70B24962-3CFF-4CA2-AFAF-D11300341556}" type="CELLRANGE">
+                    <a:fld id="{24795E42-88F6-44B3-BEEE-3629004930CD}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -413,7 +413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{742FC414-247A-4496-B7A1-8C4AD8256EDB}" type="CELLRANGE">
+                    <a:fld id="{29DBA275-8AA8-49D5-8B7C-516480190E7F}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -447,7 +447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA980B46-326F-4954-AC60-88BFD45E1D21}" type="CELLRANGE">
+                    <a:fld id="{764597D4-60EC-420C-9F6B-FF9EABDA43B5}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -548,8 +548,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.33286593647507873"/>
-                  <c:y val="-0.12959557321911216"/>
+                  <c:x val="0.42068855706508201"/>
+                  <c:y val="-0.12894035991744771"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -605,7 +605,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$5</c:f>
+              <c:f>Tabelle1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -687,7 +687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CBAB621-B228-4C6F-94EC-2F57C322B9EA}" type="CELLRANGE">
+                    <a:fld id="{BAFBB3A6-9BE2-4653-A20A-E3AC6350B17E}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -721,7 +721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D90BA106-0C7E-42F3-B6DC-074FDC474C71}" type="CELLRANGE">
+                    <a:fld id="{3D6F6A0B-A5E8-4508-8464-6A0188F74A4B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -761,7 +761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8AE71EE-73F0-4169-9E8E-D03744C7FCC1}" type="CELLRANGE">
+                    <a:fld id="{239D6B0E-02BE-4E40-A11E-4AD4FC4297A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -865,7 +865,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$8:$C$10</c:f>
+              <c:f>Tabelle1!$D$8:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -902,6 +902,163 @@
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-E9CC-435A-A74A-24A10578E016}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Actual Time for New UC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0598733448474374E-2"/>
+                  <c:y val="2.6711185308847998E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{000B2288-A898-4B5B-B4DC-67F52C1640B6}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEZ]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{000B2288-A898-4B5B-B4DC-67F52C1640B6}</c15:txfldGUID>
+                      <c15:f>Tabelle1!$A$10</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>Settings Tab (Semester II)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-C73B-47E0-9547-5402A4CCF4B8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$8:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>[h]:mm</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="2">
+                  <c:v>0.59722222222222221</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$8:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C73B-47E0-9547-5402A4CCF4B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1166,8 +1323,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.81672378387934674"/>
           <c:y val="0.44529936999366165"/>
-          <c:w val="0.17464063753688816"/>
-          <c:h val="0.2304167570625795"/>
+          <c:w val="0.18327621612065334"/>
+          <c:h val="0.27490366709169695"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1796,16 +1953,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>65890</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>580240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>20619</xdr:rowOff>
+      <xdr:rowOff>68244</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>507850</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>260200</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>20619</xdr:rowOff>
+      <xdr:rowOff>68244</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2130,20 +2287,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -2151,177 +2308,211 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="14">
         <v>0.43958333333333338</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="14">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="D2" s="4">
         <v>71.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="14">
         <v>0.33958333333333335</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="14">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="D3" s="4">
         <v>44.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="14">
         <v>0.16597222222222222</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="14">
+        <v>0.16597222222222222</v>
+      </c>
+      <c r="D4" s="4">
         <v>36.4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="14">
         <v>7.8472222222222221E-2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="14">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="D5" s="3">
         <v>15.4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="15">
-        <f>(C8-7.27)/136.01</f>
+        <f>(D8-7.27)/136.01</f>
         <v>0.29211087420042647</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="15"/>
+      <c r="D8" s="11">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="15">
-        <f t="shared" ref="B9:B10" si="0">(C9-7.27)/136.01</f>
+        <f>(D9-7.27)/136.01</f>
         <v>0.55091537386956846</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="15"/>
+      <c r="D9" s="12">
         <v>82.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="15">
-        <f t="shared" si="0"/>
+        <f>(D10-7.27)/136.01</f>
         <v>0.13623998235423868</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="15">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D10" s="12">
         <v>25.8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17"/>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="19"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="19"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="19"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="16"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>